<commit_message>
Renewable heat report update 2023
</commit_message>
<xml_diff>
--- a/Data Sources/MANUAL/RenHeatCapLA.xlsx
+++ b/Data Sources/MANUAL/RenHeatCapLA.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ische\Documents\GitHub\ScottishEnergyStatsProcessing\Data Sources\MANUAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\ScottishEnergyStatsProcessing\Data Sources\MANUAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CA93702-4686-4E67-8211-EDA2A062FB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA23AF8F-0F4F-4F31-BA57-8004A82A0244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{34935359-8B14-470A-BA1A-6155F162D50F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34935359-8B14-470A-BA1A-6155F162D50F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -606,20 +617,20 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="34.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="34.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -639,7 +650,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,19 +658,21 @@
         <v>50</v>
       </c>
       <c r="C2" s="1">
-        <v>18</v>
+        <v>59.300245142098426</v>
       </c>
       <c r="D2" s="1">
-        <v>3.5000000000000001E-3</v>
+        <f>C2/$C$35</f>
+        <v>1.0529801503213499E-2</v>
       </c>
       <c r="E2" s="1">
-        <v>0.01</v>
+        <v>9.9267978064872565E-3</v>
       </c>
       <c r="F2" s="1">
-        <v>4.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <f>E2/$E$35</f>
+        <v>4.3319047226197992E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -667,19 +680,21 @@
         <v>49</v>
       </c>
       <c r="C3" s="1">
-        <v>361</v>
+        <v>472.35065902433178</v>
       </c>
       <c r="D3" s="1">
-        <v>6.9400000000000003E-2</v>
+        <f t="shared" ref="D3:D35" si="0">C3/$C$35</f>
+        <v>8.3874167257148913E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>0.2</v>
+        <v>0.24052569297081206</v>
       </c>
       <c r="F3" s="1">
-        <v>0.1002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F3:F35" si="1">E3/$E$35</f>
+        <v>0.10496178179540905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -687,19 +702,21 @@
         <v>43</v>
       </c>
       <c r="C4" s="1">
-        <v>168</v>
+        <v>206.27609135887923</v>
       </c>
       <c r="D4" s="1">
-        <v>3.2300000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.662794802387339E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>0.06</v>
+        <v>7.4440643698485867E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>3.1699999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.2484773265109887E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -707,19 +724,21 @@
         <v>48</v>
       </c>
       <c r="C5" s="1">
-        <v>62</v>
+        <v>102.63138930362442</v>
       </c>
       <c r="D5" s="1">
-        <v>1.1900000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.8224008261291186E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>0.04</v>
+        <v>6.1815767457659786E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>1.9300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.6975467839911772E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -727,19 +746,21 @@
         <v>67</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>10.034425619606871</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.7817887551734584E-3</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>4.3496946034770109E-3</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.8981410684563546E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -747,19 +768,21 @@
         <v>66</v>
       </c>
       <c r="C7" s="1">
-        <v>293</v>
+        <v>351.10172878731328</v>
       </c>
       <c r="D7" s="1">
-        <v>5.62E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.2344287156089903E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>0.16</v>
+        <v>0.28128984803697821</v>
       </c>
       <c r="F7" s="1">
-        <v>7.8899999999999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.12275064375140961</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -767,19 +790,21 @@
         <v>42</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>53.701100862528577</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.5355749581048609E-3</v>
       </c>
       <c r="E8" s="1">
-        <v>0.01</v>
+        <v>2.2965901923440005E-2</v>
       </c>
       <c r="F8" s="1">
-        <v>2.7000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.0021972940393505E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -787,19 +812,21 @@
         <v>65</v>
       </c>
       <c r="C9" s="1">
-        <v>163</v>
+        <v>151.50694721269838</v>
       </c>
       <c r="D9" s="1">
-        <v>3.1300000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.6902723195911332E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>0.08</v>
+        <v>8.2449498555820039E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>3.9600000000000003E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.597971663512492E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -807,19 +834,21 @@
         <v>41</v>
       </c>
       <c r="C10" s="1">
-        <v>65</v>
+        <v>86.701186439763291</v>
       </c>
       <c r="D10" s="1">
-        <v>1.26E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.5395320560921166E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>0.01</v>
+        <v>2.0154739341164261E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>8.79522402260512E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -827,19 +856,21 @@
         <v>64</v>
       </c>
       <c r="C11" s="1">
-        <v>64</v>
+        <v>54.53718464232486</v>
       </c>
       <c r="D11" s="1">
-        <v>1.2200000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.6840363383270695E-3</v>
       </c>
       <c r="E11" s="1">
-        <v>0.03</v>
+        <v>3.3737503624432758E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>1.49E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.4722537330676159E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -847,19 +878,21 @@
         <v>63</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>8.5539090327510543</v>
       </c>
       <c r="D12" s="1">
-        <v>1.4E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.5188969957136047E-3</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>5.1826936637283912E-3</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.261649284638882E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -867,19 +900,21 @@
         <v>47</v>
       </c>
       <c r="C13" s="1">
-        <v>55</v>
+        <v>47.135704722896705</v>
       </c>
       <c r="D13" s="1">
-        <v>1.0699999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.3697734007145124E-3</v>
       </c>
       <c r="E13" s="1">
-        <v>0.03</v>
+        <v>1.9736773725196114E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>8.6128301367820528E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -887,19 +922,21 @@
         <v>36</v>
       </c>
       <c r="C14" s="1">
-        <v>31</v>
+        <v>10.530942327024981</v>
       </c>
       <c r="D14" s="1">
-        <v>6.0000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.8699540293576323E-3</v>
       </c>
       <c r="E14" s="1">
-        <v>0.02</v>
+        <v>5.5446761797438042E-3</v>
       </c>
       <c r="F14" s="1">
-        <v>7.9000000000000008E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.4196129906799394E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -907,19 +944,21 @@
         <v>62</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>204.72481153124102</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.6352491006422155E-2</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>0.2336242468817131</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.10195009489606109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -927,19 +966,21 @@
         <v>40</v>
       </c>
       <c r="C16" s="1">
-        <v>217</v>
+        <v>44.211779549119711</v>
       </c>
       <c r="D16" s="1">
-        <v>4.1700000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.8505790598421589E-3</v>
       </c>
       <c r="E16" s="1">
-        <v>0.25</v>
+        <v>2.8469548967120173E-2</v>
       </c>
       <c r="F16" s="1">
-        <v>0.1206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.2423681435409905E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -947,19 +988,21 @@
         <v>38</v>
       </c>
       <c r="C17" s="1">
-        <v>32</v>
+        <v>1122.5543353582025</v>
       </c>
       <c r="D17" s="1">
-        <v>6.1999999999999998E-3</v>
+        <f t="shared" si="0"/>
+        <v>0.19932926583303756</v>
       </c>
       <c r="E17" s="1">
-        <v>0.02</v>
+        <v>0.3611119565544601</v>
       </c>
       <c r="F17" s="1">
-        <v>8.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.15758380703296435</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -967,19 +1010,21 @@
         <v>61</v>
       </c>
       <c r="C18" s="1">
-        <v>996</v>
+        <v>16.720514014594261</v>
       </c>
       <c r="D18" s="1">
-        <v>0.19139999999999999</v>
+        <f t="shared" si="0"/>
+        <v>2.9690213452488057E-3</v>
       </c>
       <c r="E18" s="1">
-        <v>0.3</v>
+        <v>1.2085878771943427E-2</v>
       </c>
       <c r="F18" s="1">
-        <v>0.1469</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>5.2740950656794587E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -987,19 +1032,21 @@
         <v>60</v>
       </c>
       <c r="C19" s="1">
-        <v>15</v>
+        <v>21.536318999774704</v>
       </c>
       <c r="D19" s="1">
-        <v>2.8999999999999998E-3</v>
+        <f t="shared" si="0"/>
+        <v>3.8241522211941467E-3</v>
       </c>
       <c r="E19" s="1">
-        <v>0.01</v>
+        <v>1.350686245337584E-2</v>
       </c>
       <c r="F19" s="1">
-        <v>5.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>5.8941908952066819E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1007,19 +1054,21 @@
         <v>59</v>
       </c>
       <c r="C20" s="1">
-        <v>26</v>
+        <v>427.32468977141468</v>
       </c>
       <c r="D20" s="1">
-        <v>5.0000000000000001E-3</v>
+        <f t="shared" si="0"/>
+        <v>7.5879014495353198E-2</v>
       </c>
       <c r="E20" s="1">
-        <v>0.01</v>
+        <v>9.4336011480096377E-2</v>
       </c>
       <c r="F20" s="1">
-        <v>6.7999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.1166811454211895E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1027,19 +1076,21 @@
         <v>58</v>
       </c>
       <c r="C21" s="1">
-        <v>358</v>
+        <v>40.682621095048447</v>
       </c>
       <c r="D21" s="1">
-        <v>6.88E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.2239149051542603E-3</v>
       </c>
       <c r="E21" s="1">
-        <v>0.09</v>
+        <v>2.1994571400503645E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>4.4900000000000002E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>9.598098961940655E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1047,19 +1098,21 @@
         <v>57</v>
       </c>
       <c r="C22" s="1">
-        <v>368</v>
+        <v>370.94511443532571</v>
       </c>
       <c r="D22" s="1">
-        <v>7.0699999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.5867829285209206E-2</v>
       </c>
       <c r="E22" s="1">
-        <v>0.12</v>
+        <v>0.12388620686361766</v>
       </c>
       <c r="F22" s="1">
-        <v>5.9700000000000003E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>5.4062070673913012E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1067,19 +1120,21 @@
         <v>37</v>
       </c>
       <c r="C23" s="1">
-        <v>70</v>
+        <v>70.28142033112843</v>
       </c>
       <c r="D23" s="1">
-        <v>1.34E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.2479702295957629E-2</v>
       </c>
       <c r="E23" s="1">
-        <v>0.01</v>
+        <v>1.7758489389976276E-2</v>
       </c>
       <c r="F23" s="1">
-        <v>6.6E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>7.7495367141213042E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1087,19 +1142,21 @@
         <v>56</v>
       </c>
       <c r="C24" s="1">
-        <v>17</v>
+        <v>31.578753990313871</v>
       </c>
       <c r="D24" s="1">
-        <v>3.2000000000000002E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.607363181046196E-3</v>
       </c>
       <c r="E24" s="1">
-        <v>0.01</v>
+        <v>1.6577465964747767E-2</v>
       </c>
       <c r="F24" s="1">
-        <v>4.7999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>7.2341559183194014E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1107,19 +1164,21 @@
         <v>39</v>
       </c>
       <c r="C25" s="1">
-        <v>215</v>
+        <v>209.25143835900209</v>
       </c>
       <c r="D25" s="1">
-        <v>4.1200000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.7156273214425321E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>0.09</v>
+        <v>0.10092258930706463</v>
       </c>
       <c r="F25" s="1">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.4041094596747585E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1127,19 +1186,21 @@
         <v>46</v>
       </c>
       <c r="C26" s="1">
-        <v>29</v>
+        <v>30.201145862052531</v>
       </c>
       <c r="D26" s="1">
-        <v>5.4999999999999997E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.3627446283733456E-3</v>
       </c>
       <c r="E26" s="1">
-        <v>0.02</v>
+        <v>2.2668711662704042E-2</v>
       </c>
       <c r="F26" s="1">
-        <v>1.12E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>9.8922835965491694E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1147,19 +1208,21 @@
         <v>55</v>
       </c>
       <c r="C27" s="1">
-        <v>142</v>
+        <v>158.76953694171439</v>
       </c>
       <c r="D27" s="1">
-        <v>2.7400000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.8192323737402613E-2</v>
       </c>
       <c r="E27" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>7.8671278910769152E-2</v>
       </c>
       <c r="F27" s="1">
-        <v>3.49E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.4330958612392264E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1167,19 +1230,21 @@
         <v>54</v>
       </c>
       <c r="C28" s="1">
-        <v>37</v>
+        <v>29.028164074802728</v>
       </c>
       <c r="D28" s="1">
-        <v>7.1999999999999998E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.1544610815342342E-3</v>
       </c>
       <c r="E28" s="1">
-        <v>0.01</v>
+        <v>1.4793001534613054E-2</v>
       </c>
       <c r="F28" s="1">
-        <v>6.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>6.4554425766216485E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1187,19 +1252,21 @@
         <v>53</v>
       </c>
       <c r="C29" s="1">
-        <v>503</v>
+        <v>522.65865250441504</v>
       </c>
       <c r="D29" s="1">
-        <v>9.6600000000000005E-2</v>
+        <f t="shared" si="0"/>
+        <v>9.2807236321211975E-2</v>
       </c>
       <c r="E29" s="1">
-        <v>0.06</v>
+        <v>8.0932610781743755E-2</v>
       </c>
       <c r="F29" s="1">
-        <v>3.1399999999999997E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.5317769707193032E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1207,19 +1274,21 @@
         <v>52</v>
       </c>
       <c r="C30" s="1">
-        <v>106</v>
+        <v>119.24508429068537</v>
       </c>
       <c r="D30" s="1">
-        <v>2.0400000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.1174062009458448E-2</v>
       </c>
       <c r="E30" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>6.8964422986453638E-2</v>
       </c>
       <c r="F30" s="1">
-        <v>3.3300000000000003E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.0095033207237661E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1227,19 +1296,21 @@
         <v>51</v>
       </c>
       <c r="C31" s="1">
-        <v>574</v>
+        <v>548.49818065027785</v>
       </c>
       <c r="D31" s="1">
-        <v>0.1103</v>
+        <f t="shared" si="0"/>
+        <v>9.7395499011537268E-2</v>
       </c>
       <c r="E31" s="1">
-        <v>0.1</v>
+        <v>0.1072088794755035</v>
       </c>
       <c r="F31" s="1">
-        <v>5.0599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.6784336737795598E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1247,19 +1318,21 @@
         <v>45</v>
       </c>
       <c r="C32" s="1">
-        <v>0</v>
+        <v>6.5742290504018692</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.1673699960516187E-3</v>
       </c>
       <c r="E32" s="1">
-        <v>0</v>
+        <v>8.3239549119692516E-3</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.6324482775774128E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1267,36 +1340,40 @@
         <v>44</v>
       </c>
       <c r="C33" s="1">
-        <v>42</v>
+        <v>35.0061962168337</v>
       </c>
       <c r="D33" s="1">
-        <v>8.0999999999999996E-3</v>
+        <f t="shared" si="0"/>
+        <v>6.2159658305378541E-3</v>
       </c>
       <c r="E33" s="1">
-        <v>0.02</v>
+        <v>1.9421545766620484E-2</v>
       </c>
       <c r="F33" s="1">
-        <v>8.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>8.475269413870664E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="1">
-        <v>138</v>
+        <v>7.5039038344233155</v>
       </c>
       <c r="D34" s="1">
-        <v>2.64E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.3324501051613041E-3</v>
       </c>
       <c r="E34" s="1">
-        <v>0.1</v>
+        <v>4.1765066101823603E-3</v>
       </c>
       <c r="F34" s="1">
-        <v>4.7800000000000002E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.8225644423701601E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1304,15 +1381,17 @@
         <v>35</v>
       </c>
       <c r="C35" s="1">
-        <v>5205</v>
+        <v>5631.658405336615</v>
       </c>
       <c r="D35" s="1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E35" s="1">
-        <v>2.0299999999999998</v>
+        <v>2.2915549722626039</v>
       </c>
       <c r="F35" s="1">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>